<commit_message>
update : ip files
</commit_message>
<xml_diff>
--- a/Adressage ip/plan ip.xlsx
+++ b/Adressage ip/plan ip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwan\Desktop\Progra\Tp2AProjectMercurius\Adressage ip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01FA60F-CDA2-4A97-A088-319B6FFF5008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299C7C15-5C6E-45CE-B287-8CF1DEABA5DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1BB5A62C-880F-479D-8A61-CB9FB6A0D252}"/>
+    <workbookView xWindow="5760" yWindow="3336" windowWidth="17280" windowHeight="9024" xr2:uid="{1BB5A62C-880F-479D-8A61-CB9FB6A0D252}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>location</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Siege social</t>
+  </si>
+  <si>
+    <t>vlan centos</t>
+  </si>
+  <si>
+    <t>vlan window</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A0ECBC-2DE4-467D-BA58-C03250330E61}">
-  <dimension ref="C2:E9"/>
+  <dimension ref="C2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,9 +456,10 @@
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -462,8 +469,14 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>17</v>
       </c>
@@ -473,8 +486,14 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -484,8 +503,14 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -495,8 +520,14 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -506,8 +537,14 @@
       <c r="E6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="G6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -517,8 +554,14 @@
       <c r="E7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -528,8 +571,14 @@
       <c r="E8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>110</v>
+      </c>
+      <c r="G8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>15</v>
       </c>
@@ -538,6 +587,12 @@
       </c>
       <c r="E9" t="s">
         <v>3</v>
+      </c>
+      <c r="F9">
+        <v>130</v>
+      </c>
+      <c r="G9">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update : adressage ip
completion of the config of all the system
</commit_message>
<xml_diff>
--- a/Adressage ip/plan ip.xlsx
+++ b/Adressage ip/plan ip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwan\Desktop\Progra\Tp2AProjectMercurius\Adressage ip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691557E6-FDA8-4B5F-940E-F46B4D9B2201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753ABA47-B978-4934-89B6-2D370658DCFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3336" windowWidth="17280" windowHeight="9024" xr2:uid="{1BB5A62C-880F-479D-8A61-CB9FB6A0D252}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1BB5A62C-880F-479D-8A61-CB9FB6A0D252}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>location</t>
   </si>
@@ -94,13 +94,88 @@
   </si>
   <si>
     <t>172.13.20.0</t>
+  </si>
+  <si>
+    <t>dns</t>
+  </si>
+  <si>
+    <t>mercurius-zone-1</t>
+  </si>
+  <si>
+    <t>mercurius-zone-2</t>
+  </si>
+  <si>
+    <t>mercurius-zone-3</t>
+  </si>
+  <si>
+    <t>mercurius-zone-4</t>
+  </si>
+  <si>
+    <t>mercurius-zone-5</t>
+  </si>
+  <si>
+    <t>mercurius-zone-6</t>
+  </si>
+  <si>
+    <t>mercurius-zone-7</t>
+  </si>
+  <si>
+    <t>machine</t>
+  </si>
+  <si>
+    <t>REG1</t>
+  </si>
+  <si>
+    <t>REG2</t>
+  </si>
+  <si>
+    <t>DEP1</t>
+  </si>
+  <si>
+    <t>DEP2</t>
+  </si>
+  <si>
+    <t>DEP3</t>
+  </si>
+  <si>
+    <t>DEP4</t>
+  </si>
+  <si>
+    <t>System installer</t>
+  </si>
+  <si>
+    <t>System config</t>
+  </si>
+  <si>
+    <t>domain named</t>
+  </si>
+  <si>
+    <t>mercurius.fr</t>
+  </si>
+  <si>
+    <t>mercurius-corse.fr</t>
+  </si>
+  <si>
+    <t>mercurius-bretagne.fr</t>
+  </si>
+  <si>
+    <t>mercurius-haute-corse.fr</t>
+  </si>
+  <si>
+    <t>mercurius-finistere.fr</t>
+  </si>
+  <si>
+    <t>mercurius-corse-sud.fr</t>
+  </si>
+  <si>
+    <t>mercurius-cote-armor.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +183,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,12 +224,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,157 +564,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A0ECBC-2DE4-467D-BA58-C03250330E61}">
-  <dimension ref="C2:G9"/>
+  <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="6" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="3" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>20</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>40</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="5" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>50</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>60</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>70</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>80</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="7" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>90</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>100</v>
       </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>110</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>120</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="9" spans="3:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>130</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>140</v>
       </c>
+      <c r="H9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>